<commit_message>
better boiling ids: first water, than salt
</commit_message>
<xml_diff>
--- a/app/data/static/samples/inputs/by_department/mozzarella/План по варкам моцарелла 8 оптимизация первой варки последней линии 2.xlsx
+++ b/app/data/static/samples/inputs/by_department/mozzarella/План по варкам моцарелла 8 оптимизация первой варки последней линии 2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marklidenberg/Yandex.Disk.localized/master/code/git/2020.10-umalat/umalat/app/data/static/samples/inputs/by_department/mozzarella/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929B008F-3E0F-FA4A-BB54-9311ECE385C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB695C3A-7684-CF4C-81F9-CA6A29A004FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12209,7 +12209,7 @@
       <pane xSplit="16" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="Q1" sqref="Q1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L27" sqref="L27"/>
+      <selection pane="bottomRight" activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>